<commit_message>
holistic mean function done, visualization started
</commit_message>
<xml_diff>
--- a/data_landmark_segmented/T707C003_210728_RP0V_landmarks.xlsx
+++ b/data_landmark_segmented/T707C003_210728_RP0V_landmarks.xlsx
@@ -437,62 +437,62 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>nose_x0</t>
+          <t>nose+x0</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>nose_y0</t>
+          <t>nose+y0</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>eye_right_x0</t>
+          <t>eye_right+x0</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>eye_right_y0</t>
+          <t>eye_right+y0</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>eye_left_x0</t>
+          <t>eye_left+x0</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>eye_left_y0</t>
+          <t>eye_left+y0</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>lips_centre_x0</t>
+          <t>lips_centre+x0</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>lips_centre_y0</t>
+          <t>lips_centre+y0</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>lips_right_x0</t>
+          <t>lips_right+x0</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>lips_right_y0</t>
+          <t>lips_right+y0</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>lips_left_x0</t>
+          <t>lips_left+x0</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>lips_left_y0</t>
+          <t>lips_left+y0</t>
         </is>
       </c>
     </row>
@@ -20762,52 +20762,52 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>face_x0</t>
+          <t>face+x0</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>face_y0</t>
+          <t>face+y0</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>shoulder_right_x0</t>
+          <t>shoulder_right+x0</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>shoulder_right_y0</t>
+          <t>shoulder_right+y0</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>shoulder_left_x0</t>
+          <t>shoulder_left+x0</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>shoulder_left_y0</t>
+          <t>shoulder_left+y0</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>hand_right_x0</t>
+          <t>hand_right+x0</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>hand_right_y0</t>
+          <t>hand_right+y0</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>hand_left_x0</t>
+          <t>hand_left+x0</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>hand_left_y0</t>
+          <t>hand_left+y0</t>
         </is>
       </c>
     </row>

</xml_diff>